<commit_message>
Add command upload notebook and execute
</commit_message>
<xml_diff>
--- a/Generate_Deployment/Input_folder/PREPARE_ITEM_LIST_SI-0000_SR-00000_SR-00000_SYSTEM_Test.xlsx
+++ b/Generate_Deployment/Input_folder/PREPARE_ITEM_LIST_SI-0000_SR-00000_SR-00000_SYSTEM_Test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="6"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Howto"/>
@@ -14,13 +14,35 @@
     <sheet r:id="rId5" sheetId="5" name="U23_Import_Table_Definition"/>
     <sheet r:id="rId6" sheetId="6" name="U24_Import_Interface_Mapping"/>
     <sheet r:id="rId7" sheetId="7" name="99_Run_replace_DDL"/>
+    <sheet r:id="rId8" sheetId="8" name="ADB_Notebook_To_Shared_Folder"/>
   </sheets>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="82">
+  <si>
+    <t>SHARED_PATH</t>
+  </si>
+  <si>
+    <t>NOTEBOOK_NAME</t>
+  </si>
+  <si>
+    <t>EXECUTE_FLAG</t>
+  </si>
+  <si>
+    <t>/Shared/Execute/</t>
+  </si>
+  <si>
+    <t>Generate_Report_Something</t>
+  </si>
+  <si>
+    <t>/Shared/UTILITIES/</t>
+  </si>
+  <si>
+    <t>Generate_Job_Daily</t>
+  </si>
   <si>
     <t>TABLE_OR_VIEW_LIST</t>
   </si>
@@ -121,7 +143,7 @@
     <t>notebook_path</t>
   </si>
   <si>
-    <t>UR</t>
+    <t>UR_NO</t>
   </si>
   <si>
     <t>SI-0000_SR-00000_SR-00000_SYSTEM</t>
@@ -172,7 +194,10 @@
     <t>/Shared/Utilities/U24_Import_Interface_Mapping_Config</t>
   </si>
   <si>
-    <t>ถ้ามีแก้ไข view หรือ table ใส่ชื่อ view/table ที่ sheet 99_RUN_replace_DDL</t>
+    <t>ถ้าหากมีแก้ไข view หรือ table ใส่ชื่อ view/table ที่ sheet 99_RUN_replace_DDL</t>
+  </si>
+  <si>
+    <t>ถ้าหากมี Notebook ที่ต้องการวางใน folder /Shared/ ที่ Databricks Please Fill sheet  ADB_Notebook_To_Shared_Folder</t>
   </si>
   <si>
     <t>Sheet</t>
@@ -185,9 +210,6 @@
   </si>
   <si>
     <t>Config_List</t>
-  </si>
-  <si>
-    <t>UR_NO</t>
   </si>
   <si>
     <r>
@@ -399,6 +421,72 @@
         <family val="2"/>
       </rPr>
       <t>null</t>
+    </r>
+  </si>
+  <si>
+    <t>ADB_Notebook_To_Shared_Folder</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Path of Shared folder </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFff0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>/Shared/&lt;path&gt;/</t>
+    </r>
+  </si>
+  <si>
+    <t>The name of Notebook</t>
+  </si>
+  <si>
+    <r>
+      <t/>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFff0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> if you want to execute it, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFff0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> if you don't</t>
     </r>
   </si>
 </sst>
@@ -423,6 +511,12 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="8"/>
       <color rgb="FFc72e0f"/>
       <name val="Consolas"/>
@@ -435,12 +529,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
@@ -448,7 +536,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="18">
+  <fills count="19">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -477,7 +565,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFa9d18e"/>
+        <fgColor rgb="FFafabab"/>
       </patternFill>
     </fill>
     <fill>
@@ -487,7 +575,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFf4b183"/>
+        <fgColor rgb="FFff0000"/>
       </patternFill>
     </fill>
     <fill>
@@ -497,7 +585,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8faadc"/>
+        <fgColor rgb="FFffc000"/>
       </patternFill>
     </fill>
     <fill>
@@ -507,7 +595,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffd966"/>
+        <fgColor rgb="FFffff00"/>
       </patternFill>
     </fill>
     <fill>
@@ -517,7 +605,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFc9c9c9"/>
+        <fgColor rgb="FF92d050"/>
       </patternFill>
     </fill>
     <fill>
@@ -527,7 +615,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF8497b0"/>
+        <fgColor rgb="FF00b050"/>
       </patternFill>
     </fill>
     <fill>
@@ -535,8 +623,13 @@
         <fgColor rgb="FFd6dce5"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00b0f0"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -583,7 +676,7 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -604,7 +697,22 @@
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFc6c6c6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FFc6c6c6"/>
@@ -615,26 +723,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="41">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -644,70 +761,85 @@
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="5" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="7" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="6" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="9" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="8" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="10" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="10" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="11" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="11" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="13" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="13" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="12" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="14" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="14" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="15" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="15" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="16" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="16" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="17" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="4" applyFont="1" fillId="17" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="16" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="4" applyFont="1" fillId="16" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="4" applyFont="1" fillId="17" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="18" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="18" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -1015,154 +1147,184 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="32" width="27.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="23.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="119.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="40" width="29.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="23.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="119.29071428571429" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.1">
-      <c r="A1" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>53</v>
+      <c r="A1" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>61</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.1">
-      <c r="A2" s="16" t="s">
-        <v>54</v>
-      </c>
-      <c r="B2" s="17" t="s">
+      <c r="A2" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.1">
+      <c r="A3" s="22"/>
+      <c r="B3" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.1">
+      <c r="A4" s="22"/>
+      <c r="B4" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.1">
+      <c r="A5" s="22"/>
+      <c r="B5" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.1">
+      <c r="A6" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.1">
+      <c r="A7" s="25"/>
+      <c r="B7" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.1">
+      <c r="A8" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.1">
+      <c r="A9" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.1">
+      <c r="A10" s="30"/>
+      <c r="B10" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.1">
+      <c r="A11" s="31" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.1">
-      <c r="A3" s="18"/>
-      <c r="B3" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.1">
-      <c r="A4" s="18"/>
-      <c r="B4" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.1">
-      <c r="A5" s="18"/>
-      <c r="B5" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.1">
-      <c r="A6" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.1">
-      <c r="A7" s="21"/>
-      <c r="B7" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.1">
-      <c r="A8" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B8" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.1">
-      <c r="A9" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.1">
-      <c r="A10" s="26"/>
-      <c r="B10" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.1">
-      <c r="A11" s="27" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="28" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>67</v>
+      <c r="B11" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>74</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="20.1">
-      <c r="A12" s="29" t="s">
-        <v>68</v>
-      </c>
-      <c r="B12" s="30" t="s">
+      <c r="A12" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+      <c r="A13" s="35"/>
+      <c r="B13" s="36" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="37" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="31"/>
-      <c r="B13" s="30" t="s">
+      <c r="C14" s="21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="39"/>
+      <c r="B15" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>70</v>
+      <c r="C15" s="21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="39"/>
+      <c r="B16" s="38" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1173,127 +1335,137 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="14.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="38.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="14" width="23.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="34.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="33.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="48.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="14.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="38.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="17" width="23.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="34.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="33.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="48.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="2"/>
+      <c r="A1" s="3"/>
       <c r="B1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>32</v>
+        <v>35</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>39</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="10">
+      <c r="A2" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="13">
         <v>1</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>36</v>
+      <c r="D2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>43</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" s="10">
+      <c r="A3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="13">
         <v>1</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>40</v>
+      <c r="D3" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>47</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="C4" s="10">
+      <c r="A4" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="13">
         <v>1</v>
       </c>
-      <c r="D4" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>44</v>
+      <c r="D4" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>51</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C5" s="10">
-        <v>0</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>49</v>
+      <c r="A5" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="13">
+        <v>1</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>56</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="13"/>
-      <c r="D6" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
+      <c r="D6" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1311,78 +1483,78 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="30.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="32.29071428571429" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="24.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="30.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="32.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="24.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="4"/>
+        <v>30</v>
+      </c>
+      <c r="C1" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="4"/>
+      <c r="A2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="4"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="4"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="4"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="4"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="4"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="4"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="4"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="4"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="4"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="7"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="5"/>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1400,17 +1572,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="30.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="30.862142857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="2" t="s">
-        <v>24</v>
+      <c r="A2" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1429,56 +1601,56 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="21.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="22.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="21.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="22.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
+      <c r="A2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
+      <c r="A3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
+      <c r="A4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>20</v>
+      <c r="A5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>22</v>
+      <c r="A6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1497,22 +1669,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="34.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="34.71928571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
+      <c r="A2" s="3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
+      <c r="A3" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1527,12 +1699,91 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" style="5" width="56.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="16.290714285714284" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+      <c r="A4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+      <c r="A5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+      <c r="A6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+      <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+      <c r="A8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="0"/>
+  </sheetPr>
+  <dimension ref="A1:C3"/>
+  <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="56.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="23.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="24.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="15.719285714285713" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -1542,55 +1793,30 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
+      <c r="C3" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>